<commit_message>
docs: docstring追加 refactor: いらないコード削除
</commit_message>
<xml_diff>
--- a/result/webqsp/llama-2-70b/gpt4-llama-2-70b-comparison.xlsx
+++ b/result/webqsp/llama-2-70b/gpt4-llama-2-70b-comparison.xlsx
@@ -443,7 +443,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>question</t>
+          <t>Question</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -1898,7 +1898,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>{'Q44148', 'Q147077'}</t>
+          <t>{'Q147077', 'Q44148'}</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -2423,7 +2423,7 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>{'Q732413', 'Q8445'}</t>
+          <t>{'Q8445', 'Q732413'}</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
@@ -2973,7 +2973,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>{'Q44148', 'Q8445'}</t>
+          <t>{'Q8445', 'Q44148'}</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -2983,7 +2983,7 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>{'Q44148', 'Q8445'}</t>
+          <t>{'Q8445', 'Q44148'}</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
@@ -4128,7 +4128,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>{'Q7603534', 'Q1588'}</t>
+          <t>{'Q1588', 'Q7603534'}</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
@@ -4698,7 +4698,7 @@
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>{'Q5389', 'Q11471'}</t>
+          <t>{'Q11471', 'Q5389'}</t>
         </is>
       </c>
       <c r="G122" t="inlineStr">
@@ -4723,7 +4723,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>{'Q740126', 'Q458'}</t>
+          <t>{'Q458', 'Q740126'}</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
@@ -4733,7 +4733,7 @@
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>{'Q740126', 'Q458'}</t>
+          <t>{'Q458', 'Q740126'}</t>
         </is>
       </c>
       <c r="G123" t="inlineStr">
@@ -4838,7 +4838,7 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>{'Q44148', 'Q2041541'}</t>
+          <t>{'Q2041541', 'Q44148'}</t>
         </is>
       </c>
       <c r="G126" t="inlineStr">
@@ -5668,7 +5668,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>{'Q17738', 'Q51752'}</t>
+          <t>{'Q51752', 'Q17738'}</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
@@ -5678,7 +5678,7 @@
       </c>
       <c r="F150" t="inlineStr">
         <is>
-          <t>{'Q17738', 'Q51752'}</t>
+          <t>{'Q51752', 'Q17738'}</t>
         </is>
       </c>
       <c r="G150" t="inlineStr">
@@ -6063,7 +6063,7 @@
       </c>
       <c r="F161" t="inlineStr">
         <is>
-          <t>{'Q3115447', 'Q8445'}</t>
+          <t>{'Q8445', 'Q3115447'}</t>
         </is>
       </c>
       <c r="G161" t="inlineStr">
@@ -6098,7 +6098,7 @@
       </c>
       <c r="F162" t="inlineStr">
         <is>
-          <t>{'Q231487', 'Q8445'}</t>
+          <t>{'Q8445', 'Q231487'}</t>
         </is>
       </c>
       <c r="G162" t="inlineStr">
@@ -6193,7 +6193,7 @@
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>{'Q376880', 'Q60'}</t>
+          <t>{'Q60', 'Q376880'}</t>
         </is>
       </c>
       <c r="E165" t="inlineStr">
@@ -6203,7 +6203,7 @@
       </c>
       <c r="F165" t="inlineStr">
         <is>
-          <t>{'Q376880', 'Q1384', 'Q60'}</t>
+          <t>{'Q60', 'Q376880', 'Q1384'}</t>
         </is>
       </c>
       <c r="G165" t="inlineStr">
@@ -6683,7 +6683,7 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>{'Q6256', 'Q835309'}</t>
+          <t>{'Q835309', 'Q6256'}</t>
         </is>
       </c>
       <c r="E179" t="inlineStr">
@@ -6693,7 +6693,7 @@
       </c>
       <c r="F179" t="inlineStr">
         <is>
-          <t>{'Q6256', 'Q835309'}</t>
+          <t>{'Q835309', 'Q6256'}</t>
         </is>
       </c>
       <c r="G179" t="inlineStr">
@@ -8513,7 +8513,7 @@
       </c>
       <c r="F231" t="inlineStr">
         <is>
-          <t>{'Q66096', 'Q1397'}</t>
+          <t>{'Q1397', 'Q66096'}</t>
         </is>
       </c>
       <c r="G231" t="inlineStr">
@@ -9353,7 +9353,7 @@
       </c>
       <c r="F255" t="inlineStr">
         <is>
-          <t>{'Q280856', 'Q8445'}</t>
+          <t>{'Q8445', 'Q280856'}</t>
         </is>
       </c>
       <c r="G255" t="inlineStr">
@@ -10078,7 +10078,7 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>{'Q17738', 'Q51752'}</t>
+          <t>{'Q51752', 'Q17738'}</t>
         </is>
       </c>
       <c r="E276" t="inlineStr">
@@ -10228,7 +10228,7 @@
       </c>
       <c r="F280" t="inlineStr">
         <is>
-          <t>{'Q8445', 'Q692'}</t>
+          <t>{'Q692', 'Q8445'}</t>
         </is>
       </c>
       <c r="G280" t="inlineStr">
@@ -10918,7 +10918,7 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>{'Q66096', 'Q1408'}</t>
+          <t>{'Q1408', 'Q66096'}</t>
         </is>
       </c>
       <c r="E300" t="inlineStr">
@@ -10928,7 +10928,7 @@
       </c>
       <c r="F300" t="inlineStr">
         <is>
-          <t>{'Q66096', 'Q1408'}</t>
+          <t>{'Q1408', 'Q66096'}</t>
         </is>
       </c>
       <c r="G300" t="inlineStr">
@@ -11793,7 +11793,7 @@
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>{'Q532459', 'Q192626'}</t>
+          <t>{'Q192626', 'Q532459'}</t>
         </is>
       </c>
       <c r="E325" t="inlineStr">
@@ -11898,7 +11898,7 @@
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t>{'Q11151', 'Q1321334'}</t>
+          <t>{'Q1321334', 'Q11151'}</t>
         </is>
       </c>
       <c r="E328" t="inlineStr">
@@ -11908,7 +11908,7 @@
       </c>
       <c r="F328" t="inlineStr">
         <is>
-          <t>{'Q11151', 'Q1321334'}</t>
+          <t>{'Q1321334', 'Q11151'}</t>
         </is>
       </c>
       <c r="G328" t="inlineStr">
@@ -12119,7 +12119,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Utterance</t>
+          <t>Question</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -12654,7 +12654,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>{'Q131814', 'Q208871'}</t>
+          <t>{'Q208871', 'Q131814'}</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -12840,7 +12840,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Utterance</t>
+          <t>Question</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -13950,7 +13950,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>{'Q160071', 'Q716835'}</t>
+          <t>{'Q716835', 'Q160071'}</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -15525,7 +15525,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>{'Q362', 'Q45797'}</t>
+          <t>{'Q45797', 'Q362'}</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
@@ -15700,7 +15700,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>{'Q166150', 'Q518863'}</t>
+          <t>{'Q518863', 'Q166150'}</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">

</xml_diff>